<commit_message>
Added all reference sequences into project build
</commit_message>
<xml_diff>
--- a/tabular/HIV-1 reference sequences.xlsx
+++ b/tabular/HIV-1 reference sequences.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15900" yWindow="3640" windowWidth="25660" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="27060" yWindow="0" windowWidth="22380" windowHeight="22880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -604,11 +604,43 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="84">
+  <cellStyleXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -733,7 +765,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="84">
+  <cellStyles count="116">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -815,6 +847,38 @@
     <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1149,7 +1213,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Incorporated all pure subtype reference sequences from excel file into project build
</commit_message>
<xml_diff>
--- a/tabular/HIV-1 reference sequences.xlsx
+++ b/tabular/HIV-1 reference sequences.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27060" yWindow="0" windowWidth="22380" windowHeight="22880" tabRatio="500"/>
+    <workbookView xWindow="4660" yWindow="0" windowWidth="22380" windowHeight="28360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -604,11 +604,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="116">
+  <cellStyleXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -765,7 +777,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="116">
+  <cellStyles count="128">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -879,6 +891,18 @@
     <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1213,7 +1237,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="C29" sqref="C29:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1879,7 +1903,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>77</v>

</xml_diff>